<commit_message>
get order list service implemented and put together all services
</commit_message>
<xml_diff>
--- a/narcotics_bs.xlsx
+++ b/narcotics_bs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/firatturan/Documents/Master/Master_Firat/3.Sem/digibp/project/AS24TeamVector/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9435C8EC-8C25-4578-A3EE-577A00558239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF392BD5-8324-D349-AFE8-82910AAA43F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4830" yWindow="1245" windowWidth="22320" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="14180" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Big_Safe" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -40,9 +40,6 @@
     <t>LeftoverHandling</t>
   </si>
   <si>
-    <t>UnitsPerPackage</t>
-  </si>
-  <si>
     <t>Methadon</t>
   </si>
   <si>
@@ -91,10 +88,7 @@
     <t>BTM Team</t>
   </si>
   <si>
-    <t>PackagesInStorage</t>
-  </si>
-  <si>
-    <t>ThresholdPack</t>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -112,6 +106,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -134,18 +129,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -361,15 +353,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -389,113 +381,89 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="3">
-        <v>10</v>
-      </c>
-      <c r="H2">
-        <v>25</v>
-      </c>
-      <c r="I2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="3">
-        <v>10</v>
-      </c>
-      <c r="H3">
+      <c r="G4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="3">
-        <v>6</v>
-      </c>
-      <c r="H4">
-        <v>30</v>
-      </c>
-      <c r="I4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D5" s="2" t="b">
         <v>1</v>
@@ -504,27 +472,21 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>10</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="2" t="b">
         <v>0</v>
@@ -533,27 +495,21 @@
         <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="3">
-        <v>1</v>
-      </c>
-      <c r="H6">
+        <v>17</v>
+      </c>
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="b">
         <v>0</v>
@@ -562,16 +518,10 @@
         <v>0</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="3">
+        <v>21</v>
+      </c>
+      <c r="G7">
         <v>10</v>
-      </c>
-      <c r="H7">
-        <v>10</v>
-      </c>
-      <c r="I7">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>